<commit_message>
refactor: Arquivo xls alterado
</commit_message>
<xml_diff>
--- a/Zumbie-IA/Assets/AIData/followData.xlsx
+++ b/Zumbie-IA/Assets/AIData/followData.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr dateCompatibility="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\workspace\zumbie-ia\Zumbie-IA\Assets\AIData\"/>
@@ -16,6 +16,9 @@
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="8" uniqueCount="8">
   <si>
     <t>NAME</t>
   </si>
@@ -45,14 +48,25 @@
   </si>
   <si>
     <t>Enemy2</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -70,8 +84,8 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
+      <start/>
+      <end/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -80,11 +94,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,7 +118,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Escritório">
       <a:dk1>
@@ -222,25 +237,25 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+            <a:gs pos="0%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110%"/>
+                <a:satMod val="105%"/>
+                <a:tint val="67%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105%"/>
+                <a:satMod val="103%"/>
+                <a:tint val="73%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105%"/>
+                <a:satMod val="109%"/>
+                <a:tint val="81%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -248,25 +263,25 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+            <a:gs pos="0%">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103%"/>
+                <a:lumMod val="102%"/>
+                <a:tint val="94%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50%">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110%"/>
+                <a:lumMod val="100%"/>
+                <a:shade val="100%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100%">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99%"/>
+                <a:satMod val="120%"/>
+                <a:shade val="78%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -279,21 +294,21 @@
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:miter lim="800%"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -307,7 +322,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="63%"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -319,32 +334,32 @@
         </a:solidFill>
         <a:solidFill>
           <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
+            <a:tint val="95%"/>
+            <a:satMod val="170%"/>
           </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+            <a:gs pos="0%">
+              <a:schemeClr val="phClr">
+                <a:tint val="93%"/>
+                <a:satMod val="150%"/>
+                <a:shade val="98%"/>
+                <a:lumMod val="102%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50%">
+              <a:schemeClr val="phClr">
+                <a:tint val="98%"/>
+                <a:satMod val="130%"/>
+                <a:shade val="90%"/>
+                <a:lumMod val="103%"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100%">
+              <a:schemeClr val="phClr">
+                <a:shade val="63%"/>
+                <a:satMod val="120%"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -364,11 +379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,6 +414,9 @@
         <f xml:space="preserve"> 100</f>
         <v>100</v>
       </c>
+      <c r="C2">
+        <v>9</v>
+      </c>
       <c r="D2" t="s">
         <v>5</v>
       </c>
@@ -410,8 +428,18 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
+      <c r="C3">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: Bug de leitura de cabeçalho da tabela fixado
</commit_message>
<xml_diff>
--- a/Zumbie-IA/Assets/AIData/followData.xlsx
+++ b/Zumbie-IA/Assets/AIData/followData.xlsx
@@ -68,12 +68,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right"/>
@@ -93,7 +90,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
@@ -110,7 +110,6 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -125,7 +124,6 @@
       <c r="D2" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
@@ -141,96 +139,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-    </row>
-    <row r="15">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
refactor: Mais valores adicionados a tabela Follow
</commit_message>
<xml_diff>
--- a/Zumbie-IA/Assets/AIData/followData.xlsx
+++ b/Zumbie-IA/Assets/AIData/followData.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>NAME</t>
   </si>
@@ -35,6 +35,18 @@
   </si>
   <si>
     <t>Enemy2</t>
+  </si>
+  <si>
+    <t>&gt;10</t>
+  </si>
+  <si>
+    <t>&lt;=100</t>
+  </si>
+  <si>
+    <t>&gt;100</t>
+  </si>
+  <si>
+    <t>&gt;8</t>
   </si>
 </sst>
 </file>
@@ -130,7 +142,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -139,6 +151,34 @@
         <v>0</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: Arvore de decisões  'seguir' estavel
</commit_message>
<xml_diff>
--- a/Zumbie-IA/Assets/AIData/followData.xlsx
+++ b/Zumbie-IA/Assets/AIData/followData.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mathe\workspace\zumbie-ia\Zumbie-IA\Assets\AIData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Página1" sheetId="1" r:id="rId3"/>
+    <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>NAME</t>
   </si>
@@ -47,26 +55,35 @@
   </si>
   <si>
     <t>&gt;8</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
@@ -75,41 +92,307 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+  <a:themeElements>
+    <a:clrScheme name="Escritório">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Escritório">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Escritório">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -123,7 +406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -133,11 +416,11 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="b">
-        <v>0</v>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
@@ -147,11 +430,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="b">
-        <v>0</v>
+      <c r="D3" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -161,11 +444,11 @@
       <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="b">
-        <v>1</v>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -175,11 +458,11 @@
       <c r="C5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="1" t="b">
-        <v>1</v>
+      <c r="D5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Classificador de seguir inimigo corrigido
</commit_message>
<xml_diff>
--- a/Zumbie-IA/Assets/AIData/followData.xlsx
+++ b/Zumbie-IA/Assets/AIData/followData.xlsx
@@ -14,15 +14,12 @@
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
-  <si>
-    <t>NAME</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="13">
   <si>
     <t>LIFE</t>
   </si>
@@ -30,44 +27,44 @@
     <t>DISTANCE</t>
   </si>
   <si>
-    <t>ATTACKING</t>
-  </si>
-  <si>
-    <t>Enemy1</t>
-  </si>
-  <si>
-    <t>&gt;0</t>
-  </si>
-  <si>
     <t>&lt;=60</t>
   </si>
   <si>
-    <t>Enemy2</t>
-  </si>
-  <si>
-    <t>&gt;10</t>
-  </si>
-  <si>
-    <t>&lt;=100</t>
-  </si>
-  <si>
-    <t>&gt;100</t>
-  </si>
-  <si>
-    <t>&gt;8</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <t>true</t>
+    <t>FOLLOW</t>
+  </si>
+  <si>
+    <t>ORC</t>
+  </si>
+  <si>
+    <t>MONKEY</t>
+  </si>
+  <si>
+    <t>&gt;=50</t>
+  </si>
+  <si>
+    <t>&lt;=0</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>&gt;=60</t>
+  </si>
+  <si>
+    <t>CHARACTER_CLASS</t>
+  </si>
+  <si>
+    <t>FRIEND</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -76,6 +73,11 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,9 +100,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -383,86 +388,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>